<commit_message>
Updated description of plot tests
</commit_message>
<xml_diff>
--- a/doc/aesthetics_dynamic.xlsx
+++ b/doc/aesthetics_dynamic.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20396"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20397"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E69A9A66-01D3-4BD1-B3C5-F9664C60C82C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9E92AC7-052F-4D93-9D13-D06CD17B6DEF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="19">
   <si>
     <t>mixture</t>
   </si>
@@ -68,14 +68,31 @@
   </si>
   <si>
     <t>Combi</t>
+  </si>
+  <si>
+    <t>attributes defined in init lines (that correspond to aesth$plot) should be retrieved in plot$sit$labels</t>
+  </si>
+  <si>
+    <t>attributes defined in version lines (that correspond to aesth$version) should be retrieved in plot$sit$layers[[*]]$mapping</t>
+  </si>
+  <si>
+    <t>if group set to NULL, test group=="group" (ggplot2 default?)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -189,23 +206,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" quotePrefix="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -217,15 +228,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -239,18 +241,34 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" quotePrefix="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" quotePrefix="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -531,39 +549,39 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N11"/>
+  <dimension ref="A1:N15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="H11" sqref="H11"/>
+      <selection pane="bottomRight" activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="C1" s="14" t="s">
+      <c r="C1" s="30" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="15"/>
-      <c r="E1" s="15"/>
-      <c r="F1" s="16"/>
-      <c r="G1" s="14" t="s">
+      <c r="D1" s="31"/>
+      <c r="E1" s="31"/>
+      <c r="F1" s="32"/>
+      <c r="G1" s="30" t="s">
         <v>1</v>
       </c>
-      <c r="H1" s="15"/>
-      <c r="I1" s="15"/>
-      <c r="J1" s="16"/>
-      <c r="K1" s="14" t="s">
+      <c r="H1" s="31"/>
+      <c r="I1" s="31"/>
+      <c r="J1" s="32"/>
+      <c r="K1" s="30" t="s">
         <v>2</v>
       </c>
-      <c r="L1" s="15"/>
-      <c r="M1" s="15"/>
-      <c r="N1" s="16"/>
+      <c r="L1" s="31"/>
+      <c r="M1" s="31"/>
+      <c r="N1" s="32"/>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="C2" s="17" t="s">
+      <c r="C2" s="12" t="s">
         <v>4</v>
       </c>
       <c r="D2" s="1" t="s">
@@ -572,10 +590,10 @@
       <c r="E2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="F2" s="18" t="s">
+      <c r="F2" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="G2" s="17" t="s">
+      <c r="G2" s="12" t="s">
         <v>4</v>
       </c>
       <c r="H2" s="1" t="s">
@@ -584,10 +602,10 @@
       <c r="I2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="J2" s="18" t="s">
+      <c r="J2" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="K2" s="17" t="s">
+      <c r="K2" s="12" t="s">
         <v>4</v>
       </c>
       <c r="L2" s="1" t="s">
@@ -596,256 +614,271 @@
       <c r="M2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="N2" s="18" t="s">
+      <c r="N2" s="13" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="12" t="s">
+      <c r="B3" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="19" t="s">
+      <c r="C3" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="D3" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="E3" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="F3" s="6" t="s">
+      <c r="E3" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F3" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="G3" s="23" t="s">
-        <v>10</v>
-      </c>
-      <c r="H3" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="I3" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="J3" s="6" t="s">
+      <c r="G3" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="I3" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="J3" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="K3" s="19" t="s">
+      <c r="K3" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="L3" s="4" t="s">
+      <c r="L3" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="M3" s="4" t="s">
+      <c r="M3" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="N3" s="6" t="s">
+      <c r="N3" s="5" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A4" s="7"/>
-      <c r="B4" s="13" t="s">
+      <c r="A4" s="29"/>
+      <c r="B4" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="20" t="s">
-        <v>10</v>
-      </c>
-      <c r="D4" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="E4" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="F4" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="G4" s="21" t="s">
+      <c r="C4" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="F4" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="G4" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="H4" s="10" t="s">
+      <c r="H4" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="I4" s="10" t="s">
+      <c r="I4" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="J4" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="K4" s="20" t="s">
-        <v>10</v>
-      </c>
-      <c r="L4" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="M4" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="N4" s="11" t="s">
+      <c r="J4" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="K4" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="L4" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="M4" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="N4" s="9" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A5" s="2" t="s">
+      <c r="A5" s="28" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="12" t="s">
+      <c r="B5" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="27"/>
-      <c r="D5" s="28"/>
-      <c r="E5" s="28"/>
-      <c r="F5" s="29"/>
-      <c r="G5" s="23" t="s">
-        <v>10</v>
-      </c>
-      <c r="H5" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="I5" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="J5" s="24" t="s">
-        <v>10</v>
-      </c>
-      <c r="K5" s="19" t="s">
+      <c r="C5" s="20"/>
+      <c r="D5" s="21"/>
+      <c r="E5" s="21"/>
+      <c r="F5" s="22"/>
+      <c r="G5" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="H5" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="I5" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="J5" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="K5" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="L5" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="M5" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="N5" s="6" t="s">
+      <c r="L5" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="M5" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="N5" s="5" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A6" s="7"/>
-      <c r="B6" s="13" t="s">
+      <c r="A6" s="29"/>
+      <c r="B6" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="C6" s="30"/>
-      <c r="D6" s="31"/>
-      <c r="E6" s="31"/>
-      <c r="F6" s="32"/>
-      <c r="G6" s="21" t="s">
+      <c r="C6" s="23"/>
+      <c r="D6" s="24"/>
+      <c r="E6" s="24"/>
+      <c r="F6" s="25"/>
+      <c r="G6" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="H6" s="10" t="s">
+      <c r="H6" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="I6" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="J6" s="22" t="s">
+      <c r="I6" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="J6" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="K6" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="L6" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="K6" s="20" t="s">
+      <c r="M6" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="N6" s="9" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A7" s="28" t="s">
+        <v>2</v>
+      </c>
+      <c r="B7" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="C7" s="20"/>
+      <c r="D7" s="21"/>
+      <c r="E7" s="21"/>
+      <c r="F7" s="22"/>
+      <c r="G7" s="20"/>
+      <c r="H7" s="21"/>
+      <c r="I7" s="21"/>
+      <c r="J7" s="22"/>
+      <c r="K7" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="L6" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="M6" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="N6" s="11" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A7" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B7" s="12" t="s">
+      <c r="L7" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="M7" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="N7" s="5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A8" s="29"/>
+      <c r="B8" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="C8" s="23"/>
+      <c r="D8" s="24"/>
+      <c r="E8" s="24"/>
+      <c r="F8" s="25"/>
+      <c r="G8" s="23"/>
+      <c r="H8" s="24"/>
+      <c r="I8" s="24"/>
+      <c r="J8" s="25"/>
+      <c r="K8" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="L8" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="M8" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="N8" s="9" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="26" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C7" s="27"/>
-      <c r="D7" s="28"/>
-      <c r="E7" s="28"/>
-      <c r="F7" s="29"/>
-      <c r="G7" s="27"/>
-      <c r="H7" s="28"/>
-      <c r="I7" s="28"/>
-      <c r="J7" s="29"/>
-      <c r="K7" s="19" t="s">
-        <v>12</v>
-      </c>
-      <c r="L7" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="M7" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="N7" s="6" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A8" s="7"/>
-      <c r="B8" s="13" t="s">
+      <c r="C10" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F10" s="19" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="27"/>
+      <c r="B11" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C8" s="30"/>
-      <c r="D8" s="31"/>
-      <c r="E8" s="31"/>
-      <c r="F8" s="32"/>
-      <c r="G8" s="30"/>
-      <c r="H8" s="31"/>
-      <c r="I8" s="31"/>
-      <c r="J8" s="32"/>
-      <c r="K8" s="20" t="s">
-        <v>10</v>
-      </c>
-      <c r="L8" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="M8" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="N8" s="11" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="25" t="s">
-        <v>14</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C10" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="D10" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="E10" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="F10" s="24" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="26"/>
-      <c r="B11" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="C11" s="10" t="s">
+      <c r="C11" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="D11" s="10" t="s">
+      <c r="D11" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="E11" s="10" t="s">
+      <c r="E11" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="F11" s="22" t="s">
+      <c r="F11" s="17" t="s">
         <v>15</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A13" s="33" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A14" s="33" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A15" s="33" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>
@@ -859,5 +892,6 @@
     <mergeCell ref="A5:A6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>